<commit_message>
Doan day Doanh thu
</commit_message>
<xml_diff>
--- a/2.Design/Template/Thong_tin_ds_doanhthu.xlsx
+++ b/2.Design/Template/Thong_tin_ds_doanhthu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WMS\temp\file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038DF35C-3CF6-476C-A61A-7159CB95D326}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8ECB49-F1FD-45DE-ABE0-F20C14516727}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,18 +45,12 @@
     <t>${item.createdDate}</t>
   </si>
   <si>
-    <t>${item.createdUser}</t>
-  </si>
-  <si>
     <t>&lt;/jx:forEach&gt;</t>
   </si>
   <si>
     <t>${item.partnerName}</t>
   </si>
   <si>
-    <t>Người thực hiện</t>
-  </si>
-  <si>
     <t>Ghi chú</t>
   </si>
   <si>
@@ -127,6 +121,12 @@
   </si>
   <si>
     <t>${item.paymentRemainValue}</t>
+  </si>
+  <si>
+    <t>Ghi nhận cho</t>
+  </si>
+  <si>
+    <t>${item.userManagerName}</t>
   </si>
 </sst>
 </file>
@@ -135,7 +135,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -284,6 +284,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -299,12 +308,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -316,9 +319,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -638,7 +638,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -662,92 +662,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
+      <c r="A1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="10" t="s">
+      <c r="M2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>10</v>
+      <c r="P2" s="15" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="13"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="16"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -774,22 +774,22 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>31</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>4</v>
@@ -798,30 +798,30 @@
         <v>5</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="M5" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="N5" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -841,6 +841,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="G2:G3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="L2:L3"/>
@@ -857,7 +858,6 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
-    <mergeCell ref="G2:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>